<commit_message>
additional results with plots
</commit_message>
<xml_diff>
--- a/Results/Tables.xlsx
+++ b/Results/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\Documents\GitHub\FEM updating for VFA\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bilal\Documents\GitHub\FEM-updating-for-VFS\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C49875-526E-4108-902B-DE71F7D28529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6953EBA9-DCFC-4BE3-9FA5-F95D124C52B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="340" windowWidth="29420" windowHeight="14940" activeTab="2" xr2:uid="{AE3F04F0-B42F-45EC-9686-6EF9329B101D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{AE3F04F0-B42F-45EC-9686-6EF9329B101D}"/>
   </bookViews>
   <sheets>
     <sheet name="Beam" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ASE Wing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Mode #</t>
   </si>
@@ -134,6 +135,18 @@
   </si>
   <si>
     <t>deg</t>
+  </si>
+  <si>
+    <t>oop</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>rx</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -562,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163369B9-B44E-4A71-8613-73A8E8D0210A}">
-  <dimension ref="B4:R32"/>
+  <dimension ref="B4:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,117 +852,371 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.35">
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.92959400000000003</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1.0560799999999999</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.802145</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.88359799999999999</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0.79368700000000003</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5">
+        <v>6.1916200000000003</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4.3774199999999999</v>
+      </c>
+      <c r="G23" s="5">
+        <v>5.9538000000000002</v>
+      </c>
+      <c r="H23" s="5">
+        <v>3.73319</v>
+      </c>
+      <c r="I23" s="5">
+        <v>3.8308499999999999</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5">
+        <v>15.4815</v>
+      </c>
+      <c r="F24" s="5">
+        <v>6.0979900000000002</v>
+      </c>
+      <c r="G24" s="5">
+        <v>15.4818</v>
+      </c>
+      <c r="H24" s="5">
+        <v>11.009499999999999</v>
+      </c>
+      <c r="I24" s="5">
+        <v>10.303900000000001</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="5">
+        <v>16.644100000000002</v>
+      </c>
+      <c r="F25" s="5">
+        <v>15.244</v>
+      </c>
+      <c r="G25" s="5">
+        <v>16.369700000000002</v>
+      </c>
+      <c r="H25" s="5">
+        <v>30.261500000000002</v>
+      </c>
+      <c r="I25" s="5">
+        <v>18.9847</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5">
+        <v>37.089799999999997</v>
+      </c>
+      <c r="F26" s="5">
+        <v>35.707500000000003</v>
+      </c>
+      <c r="G26" s="5">
+        <v>36.764400000000002</v>
+      </c>
+      <c r="H26" s="5">
+        <v>39.4086</v>
+      </c>
+      <c r="I26" s="5">
+        <v>33.387799999999999</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="5">
+        <v>54.7834</v>
+      </c>
+      <c r="F27" s="5">
+        <v>51.234499999999997</v>
+      </c>
+      <c r="G27" s="5">
+        <v>54.555100000000003</v>
+      </c>
+      <c r="H27" s="5">
+        <v>52.433700000000002</v>
+      </c>
+      <c r="I27" s="5">
+        <v>52.218600000000002</v>
+      </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5">
+        <v>60.789000000000001</v>
+      </c>
+      <c r="F28" s="5">
+        <v>53.966700000000003</v>
+      </c>
+      <c r="G28" s="5">
+        <v>60.844799999999999</v>
+      </c>
+      <c r="H28" s="5">
+        <v>60.789000000000001</v>
+      </c>
+      <c r="I28" s="5">
+        <v>73.213999999999999</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5">
+        <v>81.834699999999998</v>
+      </c>
+      <c r="F29" s="5">
+        <v>79.922899999999998</v>
+      </c>
+      <c r="G29" s="5">
+        <v>81.450599999999994</v>
+      </c>
+      <c r="H29" s="5">
+        <v>78.555899999999994</v>
+      </c>
+      <c r="I29" s="5">
+        <v>77.876499999999993</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
+        <v>9</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="5">
+        <v>102.751</v>
+      </c>
+      <c r="F30" s="5">
+        <v>120.1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>102.751</v>
+      </c>
+      <c r="H30" s="5">
+        <v>116.334</v>
+      </c>
+      <c r="I30" s="5">
+        <v>108.28400000000001</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="5">
+        <v>120.971</v>
+      </c>
+      <c r="F31" s="5">
+        <v>140.959</v>
+      </c>
+      <c r="G31" s="5">
+        <v>120.60899999999999</v>
+      </c>
+      <c r="H31" s="5">
+        <v>126.926</v>
+      </c>
+      <c r="I31" s="5">
+        <v>117.88200000000001</v>
+      </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="14:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="5">
+        <v>149.34899999999999</v>
+      </c>
+      <c r="F32" s="5">
+        <v>149.16900000000001</v>
+      </c>
+      <c r="G32" s="5">
+        <v>149.16499999999999</v>
+      </c>
+      <c r="H32" s="5">
+        <v>149.19</v>
+      </c>
+      <c r="I32" s="5">
+        <v>148.18</v>
+      </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1442,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B960A5-A16E-44D8-A6DB-F7223569F15D}">
   <dimension ref="B4:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>

</xml_diff>